<commit_message>
load p&f 2020 AV data
</commit_message>
<xml_diff>
--- a/inputs/data_raw/Data_SJPF_Demographics_20200630.xlsx
+++ b/inputs/data_raw/Data_SJPF_Demographics_20200630.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Proj_CAPlans\model_SJ\inputs\data_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81CA7D2E-831D-4508-A42A-33D8AB5C1151}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3D19841-37E7-4B93-B441-B6E5F8D46FE8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="1845" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="other" sheetId="37" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="115">
   <si>
     <t>TOC</t>
   </si>
@@ -857,9 +857,6 @@
       </rPr>
       <t>$  237,229,643</t>
     </r>
-  </si>
-  <si>
-    <t>$  4,684,086</t>
   </si>
 </sst>
 </file>
@@ -867,7 +864,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0;&quot;$&quot;\-#,##0"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0;&quot;$&quot;\-#,##0"/>
   </numFmts>
   <fonts count="15">
     <font>
@@ -1293,9 +1290,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1349,86 +1343,89 @@
     <xf numFmtId="3" fontId="10" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="10" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="10" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="10" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="3" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="3" fontId="13" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="10" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="10" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="10" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="3" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="3" fontId="13" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2927,7 +2924,7 @@
   <dimension ref="A1:G55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2995,8 +2992,8 @@
       <c r="F7" s="25">
         <v>88</v>
       </c>
-      <c r="G7" s="25" t="s">
-        <v>115</v>
+      <c r="G7" s="25">
+        <v>4684086</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -3410,830 +3407,830 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="25.5">
-      <c r="C4" s="28" t="s">
+      <c r="C4" s="72" t="s">
         <v>67</v>
       </c>
-      <c r="D4" s="28"/>
-      <c r="E4" s="29" t="s">
+      <c r="D4" s="72"/>
+      <c r="E4" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="F4" s="30" t="s">
+      <c r="F4" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="G4" s="30" t="s">
+      <c r="G4" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="H4" s="30" t="s">
+      <c r="H4" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="I4" s="30" t="s">
+      <c r="I4" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="J4" s="29" t="s">
+      <c r="J4" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="K4" s="29" t="s">
+      <c r="K4" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="L4" s="31" t="s">
+      <c r="L4" s="30" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:12">
-      <c r="C5" s="32" t="s">
+      <c r="C5" s="31" t="s">
         <v>76</v>
       </c>
-      <c r="D5" s="33">
+      <c r="D5" s="32">
         <v>15</v>
       </c>
-      <c r="E5" s="34">
+      <c r="E5" s="33">
         <v>9</v>
       </c>
-      <c r="F5" s="35">
-        <v>0</v>
-      </c>
-      <c r="G5" s="35">
-        <v>0</v>
-      </c>
-      <c r="H5" s="35">
-        <v>0</v>
-      </c>
-      <c r="I5" s="35">
-        <v>0</v>
-      </c>
-      <c r="J5" s="34">
-        <v>0</v>
-      </c>
-      <c r="K5" s="34">
-        <v>0</v>
-      </c>
-      <c r="L5" s="36">
+      <c r="F5" s="34">
+        <v>0</v>
+      </c>
+      <c r="G5" s="34">
+        <v>0</v>
+      </c>
+      <c r="H5" s="34">
+        <v>0</v>
+      </c>
+      <c r="I5" s="34">
+        <v>0</v>
+      </c>
+      <c r="J5" s="33">
+        <v>0</v>
+      </c>
+      <c r="K5" s="33">
+        <v>0</v>
+      </c>
+      <c r="L5" s="35">
         <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:12">
-      <c r="C6" s="32" t="s">
+      <c r="C6" s="31" t="s">
         <v>77</v>
       </c>
-      <c r="D6" s="33">
+      <c r="D6" s="32">
         <v>46</v>
       </c>
-      <c r="E6" s="34">
+      <c r="E6" s="33">
         <v>145</v>
       </c>
-      <c r="F6" s="35">
+      <c r="F6" s="34">
         <v>4</v>
       </c>
-      <c r="G6" s="35">
-        <v>0</v>
-      </c>
-      <c r="H6" s="35">
-        <v>0</v>
-      </c>
-      <c r="I6" s="35">
-        <v>0</v>
-      </c>
-      <c r="J6" s="34">
-        <v>0</v>
-      </c>
-      <c r="K6" s="34">
-        <v>0</v>
-      </c>
-      <c r="L6" s="36">
+      <c r="G6" s="34">
+        <v>0</v>
+      </c>
+      <c r="H6" s="34">
+        <v>0</v>
+      </c>
+      <c r="I6" s="34">
+        <v>0</v>
+      </c>
+      <c r="J6" s="33">
+        <v>0</v>
+      </c>
+      <c r="K6" s="33">
+        <v>0</v>
+      </c>
+      <c r="L6" s="35">
         <v>195</v>
       </c>
     </row>
     <row r="7" spans="1:12">
-      <c r="C7" s="32" t="s">
+      <c r="C7" s="31" t="s">
         <v>78</v>
       </c>
-      <c r="D7" s="33">
+      <c r="D7" s="32">
         <v>32</v>
       </c>
-      <c r="E7" s="34">
+      <c r="E7" s="33">
         <v>148</v>
       </c>
-      <c r="F7" s="35">
+      <c r="F7" s="34">
         <v>78</v>
       </c>
-      <c r="G7" s="35">
+      <c r="G7" s="34">
         <v>3</v>
       </c>
-      <c r="H7" s="35">
-        <v>0</v>
-      </c>
-      <c r="I7" s="35">
-        <v>0</v>
-      </c>
-      <c r="J7" s="34">
-        <v>0</v>
-      </c>
-      <c r="K7" s="34">
-        <v>0</v>
-      </c>
-      <c r="L7" s="36">
+      <c r="H7" s="34">
+        <v>0</v>
+      </c>
+      <c r="I7" s="34">
+        <v>0</v>
+      </c>
+      <c r="J7" s="33">
+        <v>0</v>
+      </c>
+      <c r="K7" s="33">
+        <v>0</v>
+      </c>
+      <c r="L7" s="35">
         <v>261</v>
       </c>
     </row>
     <row r="8" spans="1:12">
-      <c r="C8" s="32" t="s">
+      <c r="C8" s="31" t="s">
         <v>79</v>
       </c>
-      <c r="D8" s="33">
+      <c r="D8" s="32">
         <v>11</v>
       </c>
-      <c r="E8" s="34">
+      <c r="E8" s="33">
         <v>62</v>
       </c>
-      <c r="F8" s="35">
+      <c r="F8" s="34">
         <v>74</v>
       </c>
-      <c r="G8" s="35">
+      <c r="G8" s="34">
         <v>94</v>
       </c>
-      <c r="H8" s="35">
+      <c r="H8" s="34">
         <v>1</v>
       </c>
-      <c r="I8" s="35">
-        <v>0</v>
-      </c>
-      <c r="J8" s="34">
-        <v>0</v>
-      </c>
-      <c r="K8" s="34">
-        <v>0</v>
-      </c>
-      <c r="L8" s="36">
+      <c r="I8" s="34">
+        <v>0</v>
+      </c>
+      <c r="J8" s="33">
+        <v>0</v>
+      </c>
+      <c r="K8" s="33">
+        <v>0</v>
+      </c>
+      <c r="L8" s="35">
         <v>242</v>
       </c>
     </row>
     <row r="9" spans="1:12">
-      <c r="C9" s="32" t="s">
+      <c r="C9" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="D9" s="33">
+      <c r="D9" s="32">
         <v>3</v>
       </c>
-      <c r="E9" s="34">
+      <c r="E9" s="33">
         <v>21</v>
       </c>
-      <c r="F9" s="35">
+      <c r="F9" s="34">
         <v>52</v>
       </c>
-      <c r="G9" s="35">
+      <c r="G9" s="34">
         <v>105</v>
       </c>
-      <c r="H9" s="35">
+      <c r="H9" s="34">
         <v>71</v>
       </c>
-      <c r="I9" s="35">
+      <c r="I9" s="34">
         <v>15</v>
       </c>
-      <c r="J9" s="34">
-        <v>0</v>
-      </c>
-      <c r="K9" s="34">
-        <v>0</v>
-      </c>
-      <c r="L9" s="36">
+      <c r="J9" s="33">
+        <v>0</v>
+      </c>
+      <c r="K9" s="33">
+        <v>0</v>
+      </c>
+      <c r="L9" s="35">
         <v>267</v>
       </c>
     </row>
     <row r="10" spans="1:12">
-      <c r="C10" s="32" t="s">
+      <c r="C10" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="D10" s="33">
+      <c r="D10" s="32">
         <v>2</v>
       </c>
-      <c r="E10" s="34">
+      <c r="E10" s="33">
         <v>8</v>
       </c>
-      <c r="F10" s="35">
+      <c r="F10" s="34">
         <v>12</v>
       </c>
-      <c r="G10" s="35">
+      <c r="G10" s="34">
         <v>62</v>
       </c>
-      <c r="H10" s="35">
+      <c r="H10" s="34">
         <v>89</v>
       </c>
-      <c r="I10" s="35">
+      <c r="I10" s="34">
         <v>148</v>
       </c>
-      <c r="J10" s="34">
+      <c r="J10" s="33">
         <v>9</v>
       </c>
-      <c r="K10" s="34">
-        <v>0</v>
-      </c>
-      <c r="L10" s="36">
+      <c r="K10" s="33">
+        <v>0</v>
+      </c>
+      <c r="L10" s="35">
         <v>330</v>
       </c>
     </row>
     <row r="11" spans="1:12">
-      <c r="C11" s="32" t="s">
+      <c r="C11" s="31" t="s">
         <v>82</v>
       </c>
-      <c r="D11" s="33">
-        <v>0</v>
-      </c>
-      <c r="E11" s="34">
+      <c r="D11" s="32">
+        <v>0</v>
+      </c>
+      <c r="E11" s="33">
         <v>2</v>
       </c>
-      <c r="F11" s="35">
+      <c r="F11" s="34">
         <v>4</v>
       </c>
-      <c r="G11" s="35">
+      <c r="G11" s="34">
         <v>27</v>
       </c>
-      <c r="H11" s="35">
+      <c r="H11" s="34">
         <v>48</v>
       </c>
-      <c r="I11" s="35">
+      <c r="I11" s="34">
         <v>178</v>
       </c>
-      <c r="J11" s="34">
+      <c r="J11" s="33">
         <v>53</v>
       </c>
-      <c r="K11" s="34">
+      <c r="K11" s="33">
         <v>1</v>
       </c>
-      <c r="L11" s="36">
+      <c r="L11" s="35">
         <v>313</v>
       </c>
     </row>
     <row r="12" spans="1:12">
-      <c r="C12" s="32" t="s">
+      <c r="C12" s="31" t="s">
         <v>83</v>
       </c>
-      <c r="D12" s="33">
-        <v>0</v>
-      </c>
-      <c r="E12" s="34">
+      <c r="D12" s="32">
+        <v>0</v>
+      </c>
+      <c r="E12" s="33">
         <v>2</v>
       </c>
-      <c r="F12" s="35">
+      <c r="F12" s="34">
         <v>1</v>
       </c>
-      <c r="G12" s="35">
+      <c r="G12" s="34">
         <v>4</v>
       </c>
-      <c r="H12" s="35">
+      <c r="H12" s="34">
         <v>14</v>
       </c>
-      <c r="I12" s="35">
+      <c r="I12" s="34">
         <v>33</v>
       </c>
-      <c r="J12" s="34">
+      <c r="J12" s="33">
         <v>16</v>
       </c>
-      <c r="K12" s="34">
+      <c r="K12" s="33">
         <v>3</v>
       </c>
-      <c r="L12" s="36">
+      <c r="L12" s="35">
         <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:12">
-      <c r="C13" s="32" t="s">
+      <c r="C13" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="D13" s="33">
-        <v>0</v>
-      </c>
-      <c r="E13" s="34">
-        <v>0</v>
-      </c>
-      <c r="F13" s="35">
-        <v>0</v>
-      </c>
-      <c r="G13" s="35">
-        <v>0</v>
-      </c>
-      <c r="H13" s="35">
+      <c r="D13" s="32">
+        <v>0</v>
+      </c>
+      <c r="E13" s="33">
+        <v>0</v>
+      </c>
+      <c r="F13" s="34">
+        <v>0</v>
+      </c>
+      <c r="G13" s="34">
+        <v>0</v>
+      </c>
+      <c r="H13" s="34">
         <v>2</v>
       </c>
-      <c r="I13" s="35">
-        <v>0</v>
-      </c>
-      <c r="J13" s="34">
+      <c r="I13" s="34">
+        <v>0</v>
+      </c>
+      <c r="J13" s="33">
         <v>2</v>
       </c>
-      <c r="K13" s="34">
-        <v>0</v>
-      </c>
-      <c r="L13" s="36">
+      <c r="K13" s="33">
+        <v>0</v>
+      </c>
+      <c r="L13" s="35">
         <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:12">
-      <c r="C14" s="32" t="s">
+      <c r="C14" s="31" t="s">
         <v>85</v>
       </c>
-      <c r="D14" s="33">
-        <v>0</v>
-      </c>
-      <c r="E14" s="34">
-        <v>0</v>
-      </c>
-      <c r="F14" s="35">
-        <v>0</v>
-      </c>
-      <c r="G14" s="35">
-        <v>0</v>
-      </c>
-      <c r="H14" s="35">
-        <v>0</v>
-      </c>
-      <c r="I14" s="35">
-        <v>0</v>
-      </c>
-      <c r="J14" s="34">
-        <v>0</v>
-      </c>
-      <c r="K14" s="34">
-        <v>0</v>
-      </c>
-      <c r="L14" s="36">
+      <c r="D14" s="32">
+        <v>0</v>
+      </c>
+      <c r="E14" s="33">
+        <v>0</v>
+      </c>
+      <c r="F14" s="34">
+        <v>0</v>
+      </c>
+      <c r="G14" s="34">
+        <v>0</v>
+      </c>
+      <c r="H14" s="34">
+        <v>0</v>
+      </c>
+      <c r="I14" s="34">
+        <v>0</v>
+      </c>
+      <c r="J14" s="33">
+        <v>0</v>
+      </c>
+      <c r="K14" s="33">
+        <v>0</v>
+      </c>
+      <c r="L14" s="35">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="15.75" thickBot="1">
-      <c r="C15" s="37" t="s">
+      <c r="C15" s="36" t="s">
         <v>86</v>
       </c>
-      <c r="D15" s="38">
-        <v>0</v>
-      </c>
-      <c r="E15" s="39">
-        <v>0</v>
-      </c>
-      <c r="F15" s="40">
-        <v>0</v>
-      </c>
-      <c r="G15" s="40">
-        <v>0</v>
-      </c>
-      <c r="H15" s="40">
-        <v>0</v>
-      </c>
-      <c r="I15" s="40">
-        <v>0</v>
-      </c>
-      <c r="J15" s="39">
-        <v>0</v>
-      </c>
-      <c r="K15" s="39">
-        <v>0</v>
-      </c>
-      <c r="L15" s="41">
+      <c r="D15" s="37">
+        <v>0</v>
+      </c>
+      <c r="E15" s="38">
+        <v>0</v>
+      </c>
+      <c r="F15" s="39">
+        <v>0</v>
+      </c>
+      <c r="G15" s="39">
+        <v>0</v>
+      </c>
+      <c r="H15" s="39">
+        <v>0</v>
+      </c>
+      <c r="I15" s="39">
+        <v>0</v>
+      </c>
+      <c r="J15" s="38">
+        <v>0</v>
+      </c>
+      <c r="K15" s="38">
+        <v>0</v>
+      </c>
+      <c r="L15" s="40">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="24.75" thickTop="1">
-      <c r="C16" s="42" t="s">
+      <c r="C16" s="41" t="s">
         <v>87</v>
       </c>
-      <c r="D16" s="43">
+      <c r="D16" s="42">
         <v>109</v>
       </c>
-      <c r="E16" s="44">
+      <c r="E16" s="43">
         <v>397</v>
       </c>
-      <c r="F16" s="45">
+      <c r="F16" s="44">
         <v>225</v>
       </c>
-      <c r="G16" s="45">
+      <c r="G16" s="44">
         <v>295</v>
       </c>
-      <c r="H16" s="45">
+      <c r="H16" s="44">
         <v>225</v>
       </c>
-      <c r="I16" s="45">
+      <c r="I16" s="44">
         <v>374</v>
       </c>
-      <c r="J16" s="44">
+      <c r="J16" s="43">
         <v>80</v>
       </c>
-      <c r="K16" s="44">
+      <c r="K16" s="43">
         <v>4</v>
       </c>
-      <c r="L16" s="46">
+      <c r="L16" s="45">
         <v>1709</v>
       </c>
     </row>
     <row r="19" spans="3:12">
-      <c r="C19" s="47" t="s">
+      <c r="C19" s="73" t="s">
         <v>67</v>
       </c>
-      <c r="D19" s="47"/>
-      <c r="E19" s="31" t="s">
+      <c r="D19" s="73"/>
+      <c r="E19" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="F19" s="31" t="s">
+      <c r="F19" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="G19" s="31" t="s">
+      <c r="G19" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="H19" s="31" t="s">
+      <c r="H19" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="I19" s="31" t="s">
+      <c r="I19" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="J19" s="31" t="s">
+      <c r="J19" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="K19" s="31" t="s">
+      <c r="K19" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="L19" s="30" t="s">
+      <c r="L19" s="29" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="20" spans="3:12">
-      <c r="C20" s="48" t="s">
+      <c r="C20" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="D20" s="49">
+      <c r="D20" s="47">
         <v>101011</v>
       </c>
-      <c r="E20" s="50">
+      <c r="E20" s="48">
         <v>109387</v>
       </c>
-      <c r="F20" s="50">
-        <v>0</v>
-      </c>
-      <c r="G20" s="50">
-        <v>0</v>
-      </c>
-      <c r="H20" s="50">
-        <v>0</v>
-      </c>
-      <c r="I20" s="50">
-        <v>0</v>
-      </c>
-      <c r="J20" s="50">
-        <v>0</v>
-      </c>
-      <c r="K20" s="50">
-        <v>0</v>
-      </c>
-      <c r="L20" s="51">
+      <c r="F20" s="48">
+        <v>0</v>
+      </c>
+      <c r="G20" s="48">
+        <v>0</v>
+      </c>
+      <c r="H20" s="48">
+        <v>0</v>
+      </c>
+      <c r="I20" s="48">
+        <v>0</v>
+      </c>
+      <c r="J20" s="48">
+        <v>0</v>
+      </c>
+      <c r="K20" s="48">
+        <v>0</v>
+      </c>
+      <c r="L20" s="49">
         <v>104152</v>
       </c>
     </row>
     <row r="21" spans="3:12">
-      <c r="C21" s="48" t="s">
+      <c r="C21" s="46" t="s">
         <v>77</v>
       </c>
-      <c r="D21" s="52">
+      <c r="D21" s="50">
         <v>101291</v>
       </c>
-      <c r="E21" s="53">
+      <c r="E21" s="51">
         <v>113917</v>
       </c>
-      <c r="F21" s="53">
+      <c r="F21" s="51">
         <v>133733</v>
       </c>
-      <c r="G21" s="36">
-        <v>0</v>
-      </c>
-      <c r="H21" s="36">
-        <v>0</v>
-      </c>
-      <c r="I21" s="36">
-        <v>0</v>
-      </c>
-      <c r="J21" s="36">
-        <v>0</v>
-      </c>
-      <c r="K21" s="36">
-        <v>0</v>
-      </c>
-      <c r="L21" s="54">
+      <c r="G21" s="35">
+        <v>0</v>
+      </c>
+      <c r="H21" s="35">
+        <v>0</v>
+      </c>
+      <c r="I21" s="35">
+        <v>0</v>
+      </c>
+      <c r="J21" s="35">
+        <v>0</v>
+      </c>
+      <c r="K21" s="35">
+        <v>0</v>
+      </c>
+      <c r="L21" s="52">
         <v>111345</v>
       </c>
     </row>
     <row r="22" spans="3:12">
-      <c r="C22" s="48" t="s">
+      <c r="C22" s="46" t="s">
         <v>78</v>
       </c>
-      <c r="D22" s="52">
+      <c r="D22" s="50">
         <v>104690</v>
       </c>
-      <c r="E22" s="53">
+      <c r="E22" s="51">
         <v>117896</v>
       </c>
-      <c r="F22" s="53">
+      <c r="F22" s="51">
         <v>139939</v>
       </c>
-      <c r="G22" s="53">
+      <c r="G22" s="51">
         <v>143138</v>
       </c>
-      <c r="H22" s="36">
-        <v>0</v>
-      </c>
-      <c r="I22" s="36">
-        <v>0</v>
-      </c>
-      <c r="J22" s="36">
-        <v>0</v>
-      </c>
-      <c r="K22" s="36">
-        <v>0</v>
-      </c>
-      <c r="L22" s="54">
+      <c r="H22" s="35">
+        <v>0</v>
+      </c>
+      <c r="I22" s="35">
+        <v>0</v>
+      </c>
+      <c r="J22" s="35">
+        <v>0</v>
+      </c>
+      <c r="K22" s="35">
+        <v>0</v>
+      </c>
+      <c r="L22" s="52">
         <v>123154</v>
       </c>
     </row>
     <row r="23" spans="3:12">
-      <c r="C23" s="48" t="s">
+      <c r="C23" s="46" t="s">
         <v>79</v>
       </c>
-      <c r="D23" s="52">
+      <c r="D23" s="50">
         <v>98188</v>
       </c>
-      <c r="E23" s="53">
+      <c r="E23" s="51">
         <v>120067</v>
       </c>
-      <c r="F23" s="53">
+      <c r="F23" s="51">
         <v>140530</v>
       </c>
-      <c r="G23" s="53">
+      <c r="G23" s="51">
         <v>148011</v>
       </c>
-      <c r="H23" s="53">
+      <c r="H23" s="51">
         <v>182350</v>
       </c>
-      <c r="I23" s="36">
-        <v>0</v>
-      </c>
-      <c r="J23" s="36">
-        <v>0</v>
-      </c>
-      <c r="K23" s="36">
-        <v>0</v>
-      </c>
-      <c r="L23" s="54">
+      <c r="I23" s="35">
+        <v>0</v>
+      </c>
+      <c r="J23" s="35">
+        <v>0</v>
+      </c>
+      <c r="K23" s="35">
+        <v>0</v>
+      </c>
+      <c r="L23" s="52">
         <v>136442</v>
       </c>
     </row>
     <row r="24" spans="3:12">
-      <c r="C24" s="48" t="s">
+      <c r="C24" s="46" t="s">
         <v>80</v>
       </c>
-      <c r="D24" s="52">
+      <c r="D24" s="50">
         <v>101516</v>
       </c>
-      <c r="E24" s="53">
+      <c r="E24" s="51">
         <v>117104</v>
       </c>
-      <c r="F24" s="53">
+      <c r="F24" s="51">
         <v>139072</v>
       </c>
-      <c r="G24" s="53">
+      <c r="G24" s="51">
         <v>147060</v>
       </c>
-      <c r="H24" s="53">
+      <c r="H24" s="51">
         <v>157655</v>
       </c>
-      <c r="I24" s="53">
+      <c r="I24" s="51">
         <v>161418</v>
       </c>
-      <c r="J24" s="36">
-        <v>0</v>
-      </c>
-      <c r="K24" s="36">
-        <v>0</v>
-      </c>
-      <c r="L24" s="54">
+      <c r="J24" s="35">
+        <v>0</v>
+      </c>
+      <c r="K24" s="35">
+        <v>0</v>
+      </c>
+      <c r="L24" s="52">
         <v>146261</v>
       </c>
     </row>
     <row r="25" spans="3:12">
-      <c r="C25" s="48" t="s">
+      <c r="C25" s="46" t="s">
         <v>81</v>
       </c>
-      <c r="D25" s="52">
+      <c r="D25" s="50">
         <v>97726</v>
       </c>
-      <c r="E25" s="53">
+      <c r="E25" s="51">
         <v>125792</v>
       </c>
-      <c r="F25" s="53">
+      <c r="F25" s="51">
         <v>143917</v>
       </c>
-      <c r="G25" s="53">
+      <c r="G25" s="51">
         <v>145332</v>
       </c>
-      <c r="H25" s="53">
+      <c r="H25" s="51">
         <v>151023</v>
       </c>
-      <c r="I25" s="53">
+      <c r="I25" s="51">
         <v>161469</v>
       </c>
-      <c r="J25" s="53">
+      <c r="J25" s="51">
         <v>172487</v>
       </c>
-      <c r="K25" s="36">
-        <v>0</v>
-      </c>
-      <c r="L25" s="54">
+      <c r="K25" s="35">
+        <v>0</v>
+      </c>
+      <c r="L25" s="52">
         <v>154031</v>
       </c>
     </row>
     <row r="26" spans="3:12">
-      <c r="C26" s="48" t="s">
+      <c r="C26" s="46" t="s">
         <v>82</v>
       </c>
-      <c r="D26" s="55">
-        <v>0</v>
-      </c>
-      <c r="E26" s="53">
+      <c r="D26" s="53">
+        <v>0</v>
+      </c>
+      <c r="E26" s="51">
         <v>137457</v>
       </c>
-      <c r="F26" s="53">
+      <c r="F26" s="51">
         <v>130011</v>
       </c>
-      <c r="G26" s="53">
+      <c r="G26" s="51">
         <v>146691</v>
       </c>
-      <c r="H26" s="53">
+      <c r="H26" s="51">
         <v>150097</v>
       </c>
-      <c r="I26" s="53">
+      <c r="I26" s="51">
         <v>158583</v>
       </c>
-      <c r="J26" s="53">
+      <c r="J26" s="51">
         <v>174150</v>
       </c>
-      <c r="K26" s="53">
+      <c r="K26" s="51">
         <v>273590</v>
       </c>
-      <c r="L26" s="54">
+      <c r="L26" s="52">
         <v>158759</v>
       </c>
     </row>
     <row r="27" spans="3:12">
-      <c r="C27" s="48" t="s">
+      <c r="C27" s="46" t="s">
         <v>83</v>
       </c>
-      <c r="D27" s="55">
-        <v>0</v>
-      </c>
-      <c r="E27" s="53">
+      <c r="D27" s="53">
+        <v>0</v>
+      </c>
+      <c r="E27" s="51">
         <v>133047</v>
       </c>
-      <c r="F27" s="53">
+      <c r="F27" s="51">
         <v>130426</v>
       </c>
-      <c r="G27" s="53">
+      <c r="G27" s="51">
         <v>148744</v>
       </c>
-      <c r="H27" s="53">
+      <c r="H27" s="51">
         <v>146776</v>
       </c>
-      <c r="I27" s="53">
+      <c r="I27" s="51">
         <v>154947</v>
       </c>
-      <c r="J27" s="53">
+      <c r="J27" s="51">
         <v>162362</v>
       </c>
-      <c r="K27" s="53">
+      <c r="K27" s="51">
         <v>158696</v>
       </c>
-      <c r="L27" s="54">
+      <c r="L27" s="52">
         <v>153883</v>
       </c>
     </row>
     <row r="28" spans="3:12">
-      <c r="C28" s="48" t="s">
+      <c r="C28" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="D28" s="55">
-        <v>0</v>
-      </c>
-      <c r="E28" s="36">
-        <v>0</v>
-      </c>
-      <c r="F28" s="36">
-        <v>0</v>
-      </c>
-      <c r="G28" s="36">
-        <v>0</v>
-      </c>
-      <c r="H28" s="53">
+      <c r="D28" s="53">
+        <v>0</v>
+      </c>
+      <c r="E28" s="35">
+        <v>0</v>
+      </c>
+      <c r="F28" s="35">
+        <v>0</v>
+      </c>
+      <c r="G28" s="35">
+        <v>0</v>
+      </c>
+      <c r="H28" s="51">
         <v>138013</v>
       </c>
-      <c r="I28" s="36">
-        <v>0</v>
-      </c>
-      <c r="J28" s="53">
+      <c r="I28" s="35">
+        <v>0</v>
+      </c>
+      <c r="J28" s="51">
         <v>170486</v>
       </c>
-      <c r="K28" s="36">
-        <v>0</v>
-      </c>
-      <c r="L28" s="54">
+      <c r="K28" s="35">
+        <v>0</v>
+      </c>
+      <c r="L28" s="52">
         <v>154250</v>
       </c>
     </row>
     <row r="29" spans="3:12">
-      <c r="C29" s="48" t="s">
+      <c r="C29" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="D29" s="55">
-        <v>0</v>
-      </c>
-      <c r="E29" s="36">
-        <v>0</v>
-      </c>
-      <c r="F29" s="36">
-        <v>0</v>
-      </c>
-      <c r="G29" s="36">
-        <v>0</v>
-      </c>
-      <c r="H29" s="36">
-        <v>0</v>
-      </c>
-      <c r="I29" s="36">
-        <v>0</v>
-      </c>
-      <c r="J29" s="36">
-        <v>0</v>
-      </c>
-      <c r="K29" s="36">
-        <v>0</v>
-      </c>
-      <c r="L29" s="35">
+      <c r="D29" s="53">
+        <v>0</v>
+      </c>
+      <c r="E29" s="35">
+        <v>0</v>
+      </c>
+      <c r="F29" s="35">
+        <v>0</v>
+      </c>
+      <c r="G29" s="35">
+        <v>0</v>
+      </c>
+      <c r="H29" s="35">
+        <v>0</v>
+      </c>
+      <c r="I29" s="35">
+        <v>0</v>
+      </c>
+      <c r="J29" s="35">
+        <v>0</v>
+      </c>
+      <c r="K29" s="35">
+        <v>0</v>
+      </c>
+      <c r="L29" s="34">
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="3:12" ht="24">
-      <c r="C30" s="56" t="s">
+      <c r="C30" s="54" t="s">
         <v>86</v>
       </c>
-      <c r="D30" s="57">
-        <v>0</v>
-      </c>
-      <c r="E30" s="58">
-        <v>0</v>
-      </c>
-      <c r="F30" s="58">
-        <v>0</v>
-      </c>
-      <c r="G30" s="58">
-        <v>0</v>
-      </c>
-      <c r="H30" s="58">
-        <v>0</v>
-      </c>
-      <c r="I30" s="58">
-        <v>0</v>
-      </c>
-      <c r="J30" s="58">
-        <v>0</v>
-      </c>
-      <c r="K30" s="58">
-        <v>0</v>
-      </c>
-      <c r="L30" s="59">
+      <c r="D30" s="55">
+        <v>0</v>
+      </c>
+      <c r="E30" s="56">
+        <v>0</v>
+      </c>
+      <c r="F30" s="56">
+        <v>0</v>
+      </c>
+      <c r="G30" s="56">
+        <v>0</v>
+      </c>
+      <c r="H30" s="56">
+        <v>0</v>
+      </c>
+      <c r="I30" s="56">
+        <v>0</v>
+      </c>
+      <c r="J30" s="56">
+        <v>0</v>
+      </c>
+      <c r="K30" s="56">
+        <v>0</v>
+      </c>
+      <c r="L30" s="57">
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="3:12" ht="24">
-      <c r="C31" s="60" t="s">
+      <c r="C31" s="58" t="s">
         <v>88</v>
       </c>
-      <c r="D31" s="61" t="s">
+      <c r="D31" s="59" t="s">
         <v>89</v>
       </c>
-      <c r="E31" s="62" t="s">
+      <c r="E31" s="60" t="s">
         <v>90</v>
       </c>
-      <c r="F31" s="62" t="s">
+      <c r="F31" s="60" t="s">
         <v>91</v>
       </c>
-      <c r="G31" s="62" t="s">
+      <c r="G31" s="60" t="s">
         <v>92</v>
       </c>
-      <c r="H31" s="62" t="s">
+      <c r="H31" s="60" t="s">
         <v>93</v>
       </c>
-      <c r="I31" s="62" t="s">
+      <c r="I31" s="60" t="s">
         <v>94</v>
       </c>
-      <c r="J31" s="62" t="s">
+      <c r="J31" s="60" t="s">
         <v>95</v>
       </c>
-      <c r="K31" s="62" t="s">
+      <c r="K31" s="60" t="s">
         <v>96</v>
       </c>
-      <c r="L31" s="63" t="s">
+      <c r="L31" s="61" t="s">
         <v>97</v>
       </c>
     </row>
@@ -4265,135 +4262,135 @@
         <v>98</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="94.5">
-      <c r="C4" s="64" t="s">
+    <row r="4" spans="1:5" ht="15.75">
+      <c r="C4" s="62" t="s">
         <v>99</v>
       </c>
-      <c r="D4" s="65" t="s">
+      <c r="D4" s="63" t="s">
         <v>100</v>
       </c>
-      <c r="E4" s="65" t="s">
+      <c r="E4" s="63" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="C5" s="66" t="s">
+      <c r="C5" s="64" t="s">
         <v>102</v>
       </c>
-      <c r="D5" s="67">
+      <c r="D5" s="65">
         <v>88</v>
       </c>
-      <c r="E5" s="68" t="s">
+      <c r="E5" s="66" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="C6" s="66" t="s">
+      <c r="C6" s="64" t="s">
         <v>104</v>
       </c>
-      <c r="D6" s="67">
+      <c r="D6" s="65">
         <v>178</v>
       </c>
-      <c r="E6" s="69">
+      <c r="E6" s="67">
         <v>16589083</v>
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="C7" s="66" t="s">
+      <c r="C7" s="64" t="s">
         <v>105</v>
       </c>
-      <c r="D7" s="67">
+      <c r="D7" s="65">
         <v>355</v>
       </c>
-      <c r="E7" s="69">
+      <c r="E7" s="67">
         <v>36241200</v>
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="C8" s="66" t="s">
+      <c r="C8" s="64" t="s">
         <v>106</v>
       </c>
-      <c r="D8" s="67">
+      <c r="D8" s="65">
         <v>351</v>
       </c>
-      <c r="E8" s="69">
+      <c r="E8" s="67">
         <v>39961460</v>
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="C9" s="66" t="s">
+      <c r="C9" s="64" t="s">
         <v>107</v>
       </c>
-      <c r="D9" s="67">
+      <c r="D9" s="65">
         <v>358</v>
       </c>
-      <c r="E9" s="69">
+      <c r="E9" s="67">
         <v>42692924</v>
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="C10" s="66" t="s">
+      <c r="C10" s="64" t="s">
         <v>108</v>
       </c>
-      <c r="D10" s="67">
+      <c r="D10" s="65">
         <v>410</v>
       </c>
-      <c r="E10" s="69">
+      <c r="E10" s="67">
         <v>44592251</v>
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="C11" s="66" t="s">
+      <c r="C11" s="64" t="s">
         <v>109</v>
       </c>
-      <c r="D11" s="67">
+      <c r="D11" s="65">
         <v>324</v>
       </c>
-      <c r="E11" s="69">
+      <c r="E11" s="67">
         <v>29022193</v>
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="C12" s="66" t="s">
+      <c r="C12" s="64" t="s">
         <v>110</v>
       </c>
-      <c r="D12" s="67">
+      <c r="D12" s="65">
         <v>192</v>
       </c>
-      <c r="E12" s="69">
+      <c r="E12" s="67">
         <v>16151991</v>
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="C13" s="66" t="s">
+      <c r="C13" s="64" t="s">
         <v>111</v>
       </c>
-      <c r="D13" s="67">
+      <c r="D13" s="65">
         <v>77</v>
       </c>
-      <c r="E13" s="69">
+      <c r="E13" s="67">
         <v>4803589</v>
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="C14" s="66" t="s">
+      <c r="C14" s="64" t="s">
         <v>112</v>
       </c>
-      <c r="D14" s="67">
+      <c r="D14" s="65">
         <v>47</v>
       </c>
-      <c r="E14" s="70">
+      <c r="E14" s="68">
         <v>2490866</v>
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="C15" s="71" t="s">
+      <c r="C15" s="69" t="s">
         <v>113</v>
       </c>
-      <c r="D15" s="72">
+      <c r="D15" s="70">
         <v>2380</v>
       </c>
-      <c r="E15" s="73" t="s">
+      <c r="E15" s="71" t="s">
         <v>114</v>
       </c>
     </row>

</xml_diff>